<commit_message>
had to update a few things
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/TestAddNewTitle.xlsx
+++ b/src/test/resources/bluesource/dataProviders/TestAddNewTitle.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\git\Java-Automation-Framework\src\test\resources\bluesource\dataProviders\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="18195" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="TestAddNewTitle" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -36,14 +31,14 @@
     <t>Add a new title as Company Admin</t>
   </si>
   <si>
-    <t>Test_COMPANY_ADMIN_Title</t>
+    <t>RANDOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,7 +619,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,10 +651,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -691,7 +685,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -867,21 +860,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>

</xml_diff>